<commit_message>
docs : data 작성 ( ~2월)
</commit_message>
<xml_diff>
--- a/docs/기능정의/DB/data.xlsx
+++ b/docs/기능정의/DB/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bumpy\docs\기능정의\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bumpy\docs\기능정의\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="193">
   <si>
     <t>stdDate</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -784,6 +784,22 @@
     <t>6,2,4순</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막 드롭 세트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15후 바로 10으로 이어서.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마지막 드롭세트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -4591,8 +4607,8 @@
   <dimension ref="A1:L658"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F122" sqref="F122"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8118,6 +8134,15 @@
       <c r="E122" s="4">
         <v>30</v>
       </c>
+      <c r="F122" s="4">
+        <v>20</v>
+      </c>
+      <c r="G122" s="4">
+        <v>10</v>
+      </c>
+      <c r="I122" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="123" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
@@ -8132,6 +8157,15 @@
       <c r="E123" s="4">
         <v>0</v>
       </c>
+      <c r="F123" s="4">
+        <v>10</v>
+      </c>
+      <c r="G123" s="4">
+        <v>10</v>
+      </c>
+      <c r="I123" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="124" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A124" s="4">
@@ -8146,6 +8180,15 @@
       <c r="E124" s="4">
         <v>70</v>
       </c>
+      <c r="F124" s="4">
+        <v>10</v>
+      </c>
+      <c r="G124" s="4">
+        <v>10</v>
+      </c>
+      <c r="I124" s="4">
+        <v>6</v>
+      </c>
       <c r="K124" s="4" t="s">
         <v>184</v>
       </c>
@@ -8160,8 +8203,20 @@
       <c r="C125" s="4" t="s">
         <v>127</v>
       </c>
+      <c r="D125" s="4">
+        <v>15</v>
+      </c>
       <c r="E125" s="4">
         <v>30</v>
+      </c>
+      <c r="F125" s="4">
+        <v>15</v>
+      </c>
+      <c r="G125" s="4">
+        <v>10</v>
+      </c>
+      <c r="I125" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
@@ -8171,8 +8226,20 @@
       <c r="C126" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="D126" s="4">
+        <v>15</v>
+      </c>
       <c r="E126" s="4">
         <v>30</v>
+      </c>
+      <c r="F126" s="4">
+        <v>15</v>
+      </c>
+      <c r="G126" s="4">
+        <v>10</v>
+      </c>
+      <c r="I126" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
@@ -8188,6 +8255,15 @@
       <c r="E127" s="4">
         <v>20</v>
       </c>
+      <c r="F127" s="4">
+        <v>10</v>
+      </c>
+      <c r="G127" s="4">
+        <v>10</v>
+      </c>
+      <c r="I127" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="128" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A128" s="4">
@@ -8202,6 +8278,15 @@
       <c r="E128" s="4">
         <v>0</v>
       </c>
+      <c r="F128" s="4">
+        <v>0</v>
+      </c>
+      <c r="G128" s="4">
+        <v>0</v>
+      </c>
+      <c r="I128" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="129" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
@@ -8219,6 +8304,15 @@
       <c r="E129" s="4">
         <v>10</v>
       </c>
+      <c r="F129" s="4">
+        <v>12</v>
+      </c>
+      <c r="G129" s="4">
+        <v>12</v>
+      </c>
+      <c r="I129" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="130" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A130" s="4">
@@ -8233,6 +8327,15 @@
       <c r="E130" s="4">
         <v>8</v>
       </c>
+      <c r="F130" s="4">
+        <v>15</v>
+      </c>
+      <c r="G130" s="4">
+        <v>10</v>
+      </c>
+      <c r="I130" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="131" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
@@ -8247,6 +8350,15 @@
       <c r="E131" s="4">
         <v>6</v>
       </c>
+      <c r="F131" s="4">
+        <v>15</v>
+      </c>
+      <c r="G131" s="4">
+        <v>10</v>
+      </c>
+      <c r="I131" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="132" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
@@ -8261,6 +8373,15 @@
       <c r="E132" s="4">
         <v>10</v>
       </c>
+      <c r="F132" s="4">
+        <v>15</v>
+      </c>
+      <c r="G132" s="4">
+        <v>10</v>
+      </c>
+      <c r="I132" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="133" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
@@ -8275,6 +8396,15 @@
       <c r="E133" s="4">
         <v>5</v>
       </c>
+      <c r="F133" s="4">
+        <v>15</v>
+      </c>
+      <c r="G133" s="4">
+        <v>15</v>
+      </c>
+      <c r="I133" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="134" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A134" s="4">
@@ -8286,8 +8416,23 @@
       <c r="C134" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="D134" s="4">
+        <v>15</v>
+      </c>
       <c r="E134" s="4">
         <v>30</v>
+      </c>
+      <c r="F134" s="4">
+        <v>12</v>
+      </c>
+      <c r="G134" s="4">
+        <v>10</v>
+      </c>
+      <c r="I134" s="4">
+        <v>5</v>
+      </c>
+      <c r="J134" s="4" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="135" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
@@ -8297,8 +8442,20 @@
       <c r="C135" s="4" t="s">
         <v>133</v>
       </c>
+      <c r="D135" s="4">
+        <v>15</v>
+      </c>
       <c r="E135" s="4">
         <v>30</v>
+      </c>
+      <c r="F135" s="4">
+        <v>12</v>
+      </c>
+      <c r="G135" s="4">
+        <v>10</v>
+      </c>
+      <c r="I135" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
@@ -8324,7 +8481,7 @@
         <v>0</v>
       </c>
       <c r="I136" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
@@ -8343,6 +8500,15 @@
       <c r="E137" s="4">
         <v>120</v>
       </c>
+      <c r="F137" s="4">
+        <v>15</v>
+      </c>
+      <c r="G137" s="4">
+        <v>10</v>
+      </c>
+      <c r="I137" s="4">
+        <v>4</v>
+      </c>
       <c r="K137" s="4" t="s">
         <v>185</v>
       </c>
@@ -8360,6 +8526,18 @@
       <c r="E138" s="4">
         <v>20</v>
       </c>
+      <c r="F138" s="4">
+        <v>15</v>
+      </c>
+      <c r="G138" s="4">
+        <v>10</v>
+      </c>
+      <c r="H138" s="4">
+        <v>20</v>
+      </c>
+      <c r="I138" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="139" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A139" s="4">
@@ -8374,6 +8552,18 @@
       <c r="E139" s="4">
         <v>35</v>
       </c>
+      <c r="F139" s="4">
+        <v>10</v>
+      </c>
+      <c r="G139" s="4">
+        <v>10</v>
+      </c>
+      <c r="I139" s="4">
+        <v>5</v>
+      </c>
+      <c r="K139" s="4" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="140" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A140" s="4">
@@ -8388,6 +8578,15 @@
       <c r="E140" s="4">
         <v>0</v>
       </c>
+      <c r="F140" s="4">
+        <v>0</v>
+      </c>
+      <c r="G140" s="4">
+        <v>0</v>
+      </c>
+      <c r="I140" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="141" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A141" s="4">
@@ -8405,6 +8604,15 @@
       <c r="E141" s="4">
         <v>0</v>
       </c>
+      <c r="F141" s="4">
+        <v>10</v>
+      </c>
+      <c r="G141" s="4">
+        <v>10</v>
+      </c>
+      <c r="I141" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="142" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A142" s="4">
@@ -8419,6 +8627,15 @@
       <c r="E142" s="4">
         <v>0</v>
       </c>
+      <c r="F142" s="4">
+        <v>10</v>
+      </c>
+      <c r="G142" s="4">
+        <v>10</v>
+      </c>
+      <c r="I142" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="143" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A143" s="4">
@@ -8428,10 +8645,19 @@
         <v>139</v>
       </c>
       <c r="D143" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E143" s="4">
         <v>35</v>
+      </c>
+      <c r="F143" s="4">
+        <v>12</v>
+      </c>
+      <c r="G143" s="4">
+        <v>10</v>
+      </c>
+      <c r="I143" s="4">
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
@@ -8447,8 +8673,17 @@
       <c r="E144" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F144" s="4">
+        <v>10</v>
+      </c>
+      <c r="G144" s="4">
+        <v>10</v>
+      </c>
+      <c r="I144" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
         <v>75</v>
       </c>
@@ -8464,8 +8699,17 @@
       <c r="E145" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F145" s="4">
+        <v>10</v>
+      </c>
+      <c r="G145" s="4">
+        <v>10</v>
+      </c>
+      <c r="I145" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
         <v>76</v>
       </c>
@@ -8478,8 +8722,17 @@
       <c r="E146" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F146" s="4">
+        <v>12</v>
+      </c>
+      <c r="G146" s="4">
+        <v>10</v>
+      </c>
+      <c r="I146" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
         <v>77</v>
       </c>
@@ -8492,8 +8745,17 @@
       <c r="E147" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F147" s="4">
+        <v>10</v>
+      </c>
+      <c r="G147" s="4">
+        <v>10</v>
+      </c>
+      <c r="I147" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A148" s="4">
         <v>78</v>
       </c>
@@ -8506,8 +8768,17 @@
       <c r="E148" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F148" s="4">
+        <v>10</v>
+      </c>
+      <c r="G148" s="4">
+        <v>10</v>
+      </c>
+      <c r="I148" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A149" s="4">
         <v>79</v>
       </c>
@@ -8523,11 +8794,20 @@
       <c r="E149" s="4">
         <v>10</v>
       </c>
+      <c r="F149" s="4">
+        <v>12</v>
+      </c>
+      <c r="G149" s="4">
+        <v>10</v>
+      </c>
       <c r="H149" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="I149" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A150" s="4">
         <v>80</v>
       </c>
@@ -8540,8 +8820,17 @@
       <c r="E150" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F150" s="4">
+        <v>12</v>
+      </c>
+      <c r="G150" s="4">
+        <v>10</v>
+      </c>
+      <c r="I150" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A151" s="4">
         <v>81</v>
       </c>
@@ -8554,8 +8843,17 @@
       <c r="E151" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F151" s="4">
+        <v>0</v>
+      </c>
+      <c r="G151" s="4">
+        <v>0</v>
+      </c>
+      <c r="I151" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A152" s="4">
         <v>82</v>
       </c>
@@ -8568,8 +8866,17 @@
       <c r="E152" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F152" s="4">
+        <v>10</v>
+      </c>
+      <c r="G152" s="4">
+        <v>10</v>
+      </c>
+      <c r="I152" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A153" s="4">
         <v>83</v>
       </c>
@@ -8585,8 +8892,17 @@
       <c r="E153" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F153" s="4">
+        <v>12</v>
+      </c>
+      <c r="G153" s="4">
+        <v>10</v>
+      </c>
+      <c r="I153" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A154" s="4">
         <v>84</v>
       </c>
@@ -8599,8 +8915,17 @@
       <c r="E154" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F154" s="4">
+        <v>10</v>
+      </c>
+      <c r="G154" s="4">
+        <v>10</v>
+      </c>
+      <c r="I154" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A155" s="4">
         <v>85</v>
       </c>
@@ -8616,8 +8941,17 @@
       <c r="E155" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F155" s="4">
+        <v>10</v>
+      </c>
+      <c r="G155" s="4">
+        <v>10</v>
+      </c>
+      <c r="I155" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A156" s="4">
         <v>86</v>
       </c>
@@ -8628,10 +8962,19 @@
         <v>4</v>
       </c>
       <c r="E156" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="F156" s="4">
+        <v>10</v>
+      </c>
+      <c r="G156" s="4">
+        <v>8</v>
+      </c>
+      <c r="I156" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A157" s="4">
         <v>87</v>
       </c>
@@ -8644,8 +8987,17 @@
       <c r="E157" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F157" s="4">
+        <v>20</v>
+      </c>
+      <c r="G157" s="4">
+        <v>15</v>
+      </c>
+      <c r="I157" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A158" s="4">
         <v>88</v>
       </c>
@@ -8658,8 +9010,17 @@
       <c r="E158" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F158" s="4">
+        <v>10</v>
+      </c>
+      <c r="G158" s="4">
+        <v>10</v>
+      </c>
+      <c r="I158" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A159" s="4">
         <v>89</v>
       </c>
@@ -8675,8 +9036,14 @@
       <c r="E159" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="F159" s="4">
+        <v>12</v>
+      </c>
+      <c r="G159" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A160" s="4">
         <v>90</v>
       </c>
@@ -8855,6 +9222,12 @@
       <c r="E171" s="4">
         <v>35</v>
       </c>
+      <c r="F171" s="4">
+        <v>12</v>
+      </c>
+      <c r="G171" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="172" spans="1:8" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A172" s="4">
@@ -9143,6 +9516,12 @@
       <c r="E189" s="4">
         <v>40</v>
       </c>
+      <c r="F189" s="4">
+        <v>12</v>
+      </c>
+      <c r="G189" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="190" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A190" s="4">
@@ -9632,6 +10011,12 @@
       <c r="C216" s="4" t="s">
         <v>139</v>
       </c>
+      <c r="D216" s="4">
+        <v>20</v>
+      </c>
+      <c r="E216" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="217" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A217" s="4">
@@ -9640,6 +10025,21 @@
       <c r="C217" s="4" t="s">
         <v>137</v>
       </c>
+      <c r="D217" s="4">
+        <v>0</v>
+      </c>
+      <c r="E217" s="4">
+        <v>0</v>
+      </c>
+      <c r="F217" s="4">
+        <v>10</v>
+      </c>
+      <c r="G217" s="4">
+        <v>10</v>
+      </c>
+      <c r="I217" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="218" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A218" s="4">
@@ -9648,6 +10048,21 @@
       <c r="C218" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="D218" s="4">
+        <v>20</v>
+      </c>
+      <c r="E218" s="4">
+        <v>30</v>
+      </c>
+      <c r="F218" s="4">
+        <v>10</v>
+      </c>
+      <c r="G218" s="4">
+        <v>10</v>
+      </c>
+      <c r="I218" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="219" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A219" s="4">
@@ -9659,6 +10074,15 @@
       <c r="C219" s="4" t="s">
         <v>115</v>
       </c>
+      <c r="D219" s="4">
+        <v>0</v>
+      </c>
+      <c r="E219" s="4">
+        <v>30</v>
+      </c>
+      <c r="H219" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="220" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A220" s="4">
@@ -9667,6 +10091,12 @@
       <c r="C220" s="4" t="s">
         <v>136</v>
       </c>
+      <c r="D220" s="4">
+        <v>20</v>
+      </c>
+      <c r="E220" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="221" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A221" s="4">
@@ -9675,6 +10105,12 @@
       <c r="C221" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="D221" s="4">
+        <v>20</v>
+      </c>
+      <c r="E221" s="4">
+        <v>35</v>
+      </c>
     </row>
     <row r="222" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A222" s="4">
@@ -9686,6 +10122,12 @@
       <c r="C222" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="D222" s="4">
+        <v>20</v>
+      </c>
+      <c r="E222" s="4">
+        <v>30</v>
+      </c>
     </row>
     <row r="223" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A223" s="4">
@@ -9694,6 +10136,12 @@
       <c r="C223" s="4" t="s">
         <v>141</v>
       </c>
+      <c r="D223" s="4">
+        <v>0</v>
+      </c>
+      <c r="E223" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="224" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A224" s="4">
@@ -9702,32 +10150,56 @@
       <c r="C224" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D224" s="4">
+        <v>0</v>
+      </c>
+      <c r="E224" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A225" s="4">
         <v>155</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D225" s="4">
+        <v>8</v>
+      </c>
+      <c r="E225" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A226" s="4">
         <v>156</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D226" s="4">
+        <v>8</v>
+      </c>
+      <c r="E226" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A227" s="4">
         <v>157</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D227" s="4">
+        <v>60</v>
+      </c>
+      <c r="E227" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A228" s="4">
         <v>158</v>
       </c>
@@ -9737,48 +10209,96 @@
       <c r="C228" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D228" s="4">
+        <v>0</v>
+      </c>
+      <c r="E228" s="4">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A229" s="4">
         <v>159</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D229" s="4">
+        <v>0</v>
+      </c>
+      <c r="E229" s="4">
+        <v>30</v>
+      </c>
+      <c r="H229" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A230" s="4">
         <v>160</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D230" s="4">
+        <v>20</v>
+      </c>
+      <c r="E230" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A231" s="4">
         <v>161</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D231" s="4">
+        <v>0</v>
+      </c>
+      <c r="E231" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A232" s="4">
         <v>162</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D232" s="4">
+        <v>0</v>
+      </c>
+      <c r="E232" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A233" s="4">
         <v>163</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D233" s="4">
+        <v>0</v>
+      </c>
+      <c r="E233" s="4">
+        <v>0</v>
+      </c>
+      <c r="F233" s="4">
+        <v>6</v>
+      </c>
+      <c r="G233" s="4">
+        <v>6</v>
+      </c>
+      <c r="I233" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A234" s="4">
         <v>164</v>
       </c>
@@ -9788,32 +10308,89 @@
       <c r="C234" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D234" s="4">
+        <v>0</v>
+      </c>
+      <c r="E234" s="4">
+        <v>0</v>
+      </c>
+      <c r="F234" s="4">
+        <v>8</v>
+      </c>
+      <c r="G234" s="4">
+        <v>8</v>
+      </c>
+      <c r="I234" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A235" s="4">
         <v>165</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D235" s="4">
+        <v>60</v>
+      </c>
+      <c r="E235" s="4">
+        <v>50</v>
+      </c>
+      <c r="F235" s="4">
+        <v>10</v>
+      </c>
+      <c r="G235" s="4">
+        <v>8</v>
+      </c>
+      <c r="I235" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A236" s="4">
         <v>166</v>
       </c>
       <c r="C236" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D236" s="4">
+        <v>20</v>
+      </c>
+      <c r="E236" s="4">
+        <v>30</v>
+      </c>
+      <c r="F236" s="4">
+        <v>10</v>
+      </c>
+      <c r="G236" s="4">
+        <v>10</v>
+      </c>
+      <c r="I236" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A237" s="4">
         <v>167</v>
       </c>
       <c r="C237" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D237" s="4">
+        <v>0</v>
+      </c>
+      <c r="E237" s="4">
+        <v>20</v>
+      </c>
+      <c r="H237" s="4">
+        <v>20</v>
+      </c>
+      <c r="I237" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A238" s="4">
         <v>168</v>
       </c>
@@ -9823,40 +10400,121 @@
       <c r="C238" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D238" s="4">
+        <v>0</v>
+      </c>
+      <c r="E238" s="4">
+        <v>10</v>
+      </c>
+      <c r="F238" s="4">
+        <v>10</v>
+      </c>
+      <c r="G238" s="4">
+        <v>8</v>
+      </c>
+      <c r="H238" s="4">
+        <v>20</v>
+      </c>
+      <c r="I238" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A239" s="4">
         <v>169</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D239" s="4">
+        <v>20</v>
+      </c>
+      <c r="E239" s="4">
+        <v>35</v>
+      </c>
+      <c r="F239" s="4">
+        <v>10</v>
+      </c>
+      <c r="G239" s="4">
+        <v>8</v>
+      </c>
+      <c r="I239" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A240" s="4">
         <v>170</v>
       </c>
       <c r="C240" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D240" s="4">
+        <v>15</v>
+      </c>
+      <c r="E240" s="4">
+        <v>10</v>
+      </c>
+      <c r="F240" s="4">
+        <v>10</v>
+      </c>
+      <c r="G240" s="4">
+        <v>20</v>
+      </c>
+      <c r="I240" s="4">
+        <v>5</v>
+      </c>
+      <c r="K240" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A241" s="4">
         <v>171</v>
       </c>
       <c r="C241" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D241" s="4">
+        <v>30</v>
+      </c>
+      <c r="E241" s="4">
+        <v>30</v>
+      </c>
+      <c r="F241" s="4">
+        <v>10</v>
+      </c>
+      <c r="G241" s="4">
+        <v>10</v>
+      </c>
+      <c r="I241" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A242" s="4">
         <v>172</v>
       </c>
       <c r="C242" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="243" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D242" s="4">
+        <v>0</v>
+      </c>
+      <c r="E242" s="4">
+        <v>0</v>
+      </c>
+      <c r="F242" s="4">
+        <v>10</v>
+      </c>
+      <c r="G242" s="4">
+        <v>10</v>
+      </c>
+      <c r="I242" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A243" s="4">
         <v>173</v>
       </c>
@@ -9866,40 +10524,118 @@
       <c r="C243" s="4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D243" s="4">
+        <v>20</v>
+      </c>
+      <c r="E243" s="4">
+        <v>40</v>
+      </c>
+      <c r="F243" s="4">
+        <v>12</v>
+      </c>
+      <c r="G243" s="4">
+        <v>8</v>
+      </c>
+      <c r="I243" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A244" s="4">
         <v>174</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="245" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D244" s="4">
+        <v>20</v>
+      </c>
+      <c r="E244" s="4">
+        <v>40</v>
+      </c>
+      <c r="F244" s="4">
+        <v>12</v>
+      </c>
+      <c r="G244" s="4">
+        <v>8</v>
+      </c>
+      <c r="I244" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A245" s="4">
         <v>175</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D245" s="4">
+        <v>0</v>
+      </c>
+      <c r="E245" s="4">
+        <v>15</v>
+      </c>
+      <c r="F245" s="4">
+        <v>10</v>
+      </c>
+      <c r="G245" s="4">
+        <v>10</v>
+      </c>
+      <c r="H245" s="4">
+        <v>20</v>
+      </c>
+      <c r="I245" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A246" s="4">
         <v>176</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="247" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D246" s="4">
+        <v>0</v>
+      </c>
+      <c r="E246" s="4">
+        <v>0</v>
+      </c>
+      <c r="F246" s="4">
+        <v>15</v>
+      </c>
+      <c r="G246" s="4">
+        <v>10</v>
+      </c>
+      <c r="I246" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A247" s="4">
         <v>177</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="248" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D247" s="4">
+        <v>0</v>
+      </c>
+      <c r="E247" s="4">
+        <v>0</v>
+      </c>
+      <c r="F247" s="4">
+        <v>12</v>
+      </c>
+      <c r="G247" s="4">
+        <v>12</v>
+      </c>
+      <c r="I247" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A248" s="4">
         <v>178</v>
       </c>
@@ -9909,32 +10645,98 @@
       <c r="C248" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="249" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D248" s="4">
+        <v>20</v>
+      </c>
+      <c r="E248" s="4">
+        <v>40</v>
+      </c>
+      <c r="F248" s="4">
+        <v>10</v>
+      </c>
+      <c r="G248" s="4">
+        <v>10</v>
+      </c>
+      <c r="I248" s="4">
+        <v>6</v>
+      </c>
+      <c r="K248" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A249" s="4">
         <v>179</v>
       </c>
       <c r="C249" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="250" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D249" s="4">
+        <v>0</v>
+      </c>
+      <c r="E249" s="4">
+        <v>20</v>
+      </c>
+      <c r="F249" s="4">
+        <v>10</v>
+      </c>
+      <c r="G249" s="4">
+        <v>10</v>
+      </c>
+      <c r="H249" s="4">
+        <v>20</v>
+      </c>
+      <c r="I249" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A250" s="4">
         <v>180</v>
       </c>
       <c r="C250" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="251" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D250" s="4">
+        <v>0</v>
+      </c>
+      <c r="E250" s="4">
+        <v>0</v>
+      </c>
+      <c r="F250" s="4">
+        <v>0</v>
+      </c>
+      <c r="G250" s="4">
+        <v>0</v>
+      </c>
+      <c r="I250" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A251" s="4">
         <v>181</v>
       </c>
       <c r="C251" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="252" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D251" s="4">
+        <v>0</v>
+      </c>
+      <c r="E251" s="4">
+        <v>0</v>
+      </c>
+      <c r="F251" s="4">
+        <v>15</v>
+      </c>
+      <c r="G251" s="4">
+        <v>15</v>
+      </c>
+      <c r="I251" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A252" s="4">
         <v>182</v>
       </c>
@@ -9944,40 +10746,121 @@
       <c r="C252" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="253" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D252" s="4">
+        <v>0</v>
+      </c>
+      <c r="E252" s="4">
+        <v>30</v>
+      </c>
+      <c r="F252" s="4">
+        <v>10</v>
+      </c>
+      <c r="G252" s="4">
+        <v>8</v>
+      </c>
+      <c r="H252" s="4">
+        <v>20</v>
+      </c>
+      <c r="I252" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A253" s="4">
         <v>183</v>
       </c>
       <c r="C253" s="4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="254" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D253" s="4">
+        <v>0</v>
+      </c>
+      <c r="E253" s="4">
+        <v>10</v>
+      </c>
+      <c r="F253" s="4">
+        <v>10</v>
+      </c>
+      <c r="G253" s="4">
+        <v>10</v>
+      </c>
+      <c r="H253" s="4">
+        <v>20</v>
+      </c>
+      <c r="I253" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A254" s="4">
         <v>184</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="255" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D254" s="4">
+        <v>0</v>
+      </c>
+      <c r="E254" s="4">
+        <v>0</v>
+      </c>
+      <c r="F254" s="4">
+        <v>10</v>
+      </c>
+      <c r="G254" s="4">
+        <v>10</v>
+      </c>
+      <c r="I254" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A255" s="4">
         <v>185</v>
       </c>
       <c r="C255" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D255" s="4">
+        <v>25</v>
+      </c>
+      <c r="E255" s="4">
+        <v>30</v>
+      </c>
+      <c r="F255" s="4">
+        <v>10</v>
+      </c>
+      <c r="G255" s="4">
+        <v>10</v>
+      </c>
+      <c r="I255" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A256" s="4">
         <v>186</v>
       </c>
       <c r="C256" s="4" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D256" s="4">
+        <v>0</v>
+      </c>
+      <c r="E256" s="4">
+        <v>0</v>
+      </c>
+      <c r="F256" s="4">
+        <v>12</v>
+      </c>
+      <c r="G256" s="4">
+        <v>12</v>
+      </c>
+      <c r="I256" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A257" s="4">
         <v>187</v>
       </c>
@@ -9987,56 +10870,161 @@
       <c r="C257" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="258" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D257" s="4">
+        <v>10</v>
+      </c>
+      <c r="E257" s="4">
+        <v>10</v>
+      </c>
+      <c r="F257" s="4">
+        <v>10</v>
+      </c>
+      <c r="G257" s="4">
+        <v>10</v>
+      </c>
+      <c r="I257" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A258" s="4">
         <v>188</v>
       </c>
       <c r="C258" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="259" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D258" s="4">
+        <v>8</v>
+      </c>
+      <c r="E258" s="4">
+        <v>8</v>
+      </c>
+      <c r="F258" s="4">
+        <v>10</v>
+      </c>
+      <c r="G258" s="4">
+        <v>10</v>
+      </c>
+      <c r="I258" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A259" s="4">
         <v>189</v>
       </c>
       <c r="C259" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="260" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D259" s="4">
+        <v>8</v>
+      </c>
+      <c r="E259" s="4">
+        <v>8</v>
+      </c>
+      <c r="F259" s="4">
+        <v>10</v>
+      </c>
+      <c r="G259" s="4">
+        <v>10</v>
+      </c>
+      <c r="I259" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A260" s="4">
         <v>190</v>
       </c>
       <c r="C260" s="4" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D260" s="4">
+        <v>0</v>
+      </c>
+      <c r="E260" s="4">
+        <v>0</v>
+      </c>
+      <c r="F260" s="4">
+        <v>15</v>
+      </c>
+      <c r="G260" s="4">
+        <v>15</v>
+      </c>
+      <c r="I260" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A261" s="4">
         <v>191</v>
       </c>
       <c r="C261" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D261" s="4">
+        <v>0</v>
+      </c>
+      <c r="E261" s="4">
+        <v>0</v>
+      </c>
+      <c r="F261" s="4">
+        <v>10</v>
+      </c>
+      <c r="G261" s="4">
+        <v>10</v>
+      </c>
+      <c r="I261" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A262" s="4">
         <v>192</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="263" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D262" s="4">
+        <v>15</v>
+      </c>
+      <c r="E262" s="4">
+        <v>15</v>
+      </c>
+      <c r="F262" s="4">
+        <v>10</v>
+      </c>
+      <c r="G262" s="4">
+        <v>10</v>
+      </c>
+      <c r="I262" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A263" s="4">
         <v>193</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D263" s="4">
+        <v>0</v>
+      </c>
+      <c r="E263" s="4">
+        <v>0</v>
+      </c>
+      <c r="F263" s="4">
+        <v>15</v>
+      </c>
+      <c r="G263" s="4">
+        <v>15</v>
+      </c>
+      <c r="I263" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A264" s="4">
         <v>194</v>
       </c>
@@ -10046,40 +11034,121 @@
       <c r="C264" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="265" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D264" s="4">
+        <v>0</v>
+      </c>
+      <c r="E264" s="4">
+        <v>15</v>
+      </c>
+      <c r="F264" s="4">
+        <v>10</v>
+      </c>
+      <c r="G264" s="4">
+        <v>8</v>
+      </c>
+      <c r="H264" s="4">
+        <v>20</v>
+      </c>
+      <c r="I264" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A265" s="4">
         <v>195</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="266" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D265" s="4">
+        <v>0</v>
+      </c>
+      <c r="E265" s="4">
+        <v>10</v>
+      </c>
+      <c r="F265" s="4">
+        <v>10</v>
+      </c>
+      <c r="G265" s="4">
+        <v>8</v>
+      </c>
+      <c r="H265" s="4">
+        <v>20</v>
+      </c>
+      <c r="I265" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A266" s="4">
         <v>196</v>
       </c>
       <c r="C266" s="4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D266" s="4">
+        <v>20</v>
+      </c>
+      <c r="E266" s="4">
+        <v>30</v>
+      </c>
+      <c r="F266" s="4">
+        <v>12</v>
+      </c>
+      <c r="G266" s="4">
+        <v>10</v>
+      </c>
+      <c r="I266" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A267" s="4">
         <v>197</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D267" s="4">
+        <v>15</v>
+      </c>
+      <c r="E267" s="4">
+        <v>15</v>
+      </c>
+      <c r="F267" s="4">
+        <v>20</v>
+      </c>
+      <c r="G267" s="4">
+        <v>15</v>
+      </c>
+      <c r="I267" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A268" s="4">
         <v>198</v>
       </c>
       <c r="C268" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="269" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D268" s="4">
+        <v>10</v>
+      </c>
+      <c r="E268" s="4">
+        <v>10</v>
+      </c>
+      <c r="F268" s="4">
+        <v>10</v>
+      </c>
+      <c r="G268" s="4">
+        <v>10</v>
+      </c>
+      <c r="I268" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A269" s="4">
         <v>199</v>
       </c>
@@ -10089,40 +11158,121 @@
       <c r="C269" s="4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D269" s="4">
+        <v>0</v>
+      </c>
+      <c r="E269" s="4">
+        <v>10</v>
+      </c>
+      <c r="F269" s="4">
+        <v>10</v>
+      </c>
+      <c r="G269" s="4">
+        <v>10</v>
+      </c>
+      <c r="H269" s="4">
+        <v>20</v>
+      </c>
+      <c r="I269" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A270" s="4">
         <v>200</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="271" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D270" s="4">
+        <v>0</v>
+      </c>
+      <c r="E270" s="4">
+        <v>20</v>
+      </c>
+      <c r="F270" s="4">
+        <v>10</v>
+      </c>
+      <c r="G270" s="4">
+        <v>8</v>
+      </c>
+      <c r="H270" s="4">
+        <v>20</v>
+      </c>
+      <c r="I270" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A271" s="4">
         <v>201</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="272" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D271" s="4">
+        <v>50</v>
+      </c>
+      <c r="E271" s="4">
+        <v>50</v>
+      </c>
+      <c r="F271" s="4">
+        <v>10</v>
+      </c>
+      <c r="G271" s="4">
+        <v>10</v>
+      </c>
+      <c r="I271" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A272" s="4">
         <v>202</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D272" s="4">
+        <v>30</v>
+      </c>
+      <c r="E272" s="4">
+        <v>35</v>
+      </c>
+      <c r="F272" s="4">
+        <v>10</v>
+      </c>
+      <c r="G272" s="4">
+        <v>10</v>
+      </c>
+      <c r="I272" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A273" s="4">
         <v>203</v>
       </c>
       <c r="C273" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="D273" s="4">
+        <v>0</v>
+      </c>
+      <c r="E273" s="4">
+        <v>0</v>
+      </c>
+      <c r="F273" s="4">
+        <v>10</v>
+      </c>
+      <c r="G273" s="4">
+        <v>10</v>
+      </c>
+      <c r="I273" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A274" s="4">
         <v>204</v>
       </c>
@@ -10133,7 +11283,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="275" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A275" s="4">
         <v>205</v>
       </c>
@@ -10141,7 +11291,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="276" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A276" s="4">
         <v>206</v>
       </c>
@@ -10149,7 +11299,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="277" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A277" s="4">
         <v>207</v>
       </c>
@@ -10157,7 +11307,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A278" s="4">
         <v>208</v>
       </c>
@@ -10168,7 +11318,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A279" s="4">
         <v>209</v>
       </c>
@@ -10176,7 +11326,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A280" s="4">
         <v>210</v>
       </c>
@@ -10184,7 +11334,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="281" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A281" s="4">
         <v>211</v>
       </c>
@@ -10192,7 +11342,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A282" s="4">
         <v>212</v>
       </c>
@@ -10203,7 +11353,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A283" s="4">
         <v>213</v>
       </c>
@@ -10211,7 +11361,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A284" s="4">
         <v>214</v>
       </c>
@@ -10219,7 +11369,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="285" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A285" s="4">
         <v>215</v>
       </c>
@@ -10227,7 +11377,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A286" s="4">
         <v>216</v>
       </c>
@@ -10238,7 +11388,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A287" s="4">
         <v>217</v>
       </c>
@@ -10246,7 +11396,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="288" spans="1:3" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A288" s="4">
         <v>218</v>
       </c>

</xml_diff>